<commit_message>
get data to model
</commit_message>
<xml_diff>
--- a/smartMeter/sourceData2/bus3I1.xlsx
+++ b/smartMeter/sourceData2/bus3I1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="215">
   <si>
     <t>当前表型:国网表</t>
   </si>
@@ -661,9 +661,6 @@
   </si>
   <si>
     <t>2015/10/27 16:07:22</t>
-  </si>
-  <si>
-    <t>2015/10/27 16:07:27</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174:G176"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
@@ -3949,21 +3948,8 @@
       </c>
     </row>
     <row r="174" spans="1:5">
-      <c r="A174">
-        <v>709148</v>
-      </c>
-      <c r="B174">
-        <v>131009003274</v>
-      </c>
-      <c r="C174" t="s">
-        <v>7</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>